<commit_message>
moved all input parameters to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
+++ b/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
   <si>
     <t>Username</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Product2 Name</t>
   </si>
   <si>
-    <t>Product Quantity</t>
-  </si>
-  <si>
     <t>Quote Record Type</t>
   </si>
   <si>
@@ -212,6 +209,147 @@
   </si>
   <si>
     <t>CoxAuto123</t>
+  </si>
+  <si>
+    <t>Urgent Request</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Ownership Change</t>
+  </si>
+  <si>
+    <t>TestAutomationDemoNew1</t>
+  </si>
+  <si>
+    <t>Existing Dealer Group</t>
+  </si>
+  <si>
+    <t>Dealer Group Account</t>
+  </si>
+  <si>
+    <t>Test Customer 1</t>
+  </si>
+  <si>
+    <t>Dealer Type</t>
+  </si>
+  <si>
+    <t>Franchise</t>
+  </si>
+  <si>
+    <t>Customer's Website URL</t>
+  </si>
+  <si>
+    <t>www.testAutomation.com</t>
+  </si>
+  <si>
+    <t>Customer Type</t>
+  </si>
+  <si>
+    <t>Dealer</t>
+  </si>
+  <si>
+    <t>Lot Size - New</t>
+  </si>
+  <si>
+    <t>Lot Size - Used</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Physical Location Phone</t>
+  </si>
+  <si>
+    <t>Physical Location Street 1</t>
+  </si>
+  <si>
+    <t>Physical Location City</t>
+  </si>
+  <si>
+    <t>Physical Location State</t>
+  </si>
+  <si>
+    <t>Physical Location Postal Code</t>
+  </si>
+  <si>
+    <t>Billing Address same as Physical?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>111-222-3333</t>
+  </si>
+  <si>
+    <t>111 Summit Trl</t>
+  </si>
+  <si>
+    <t>Dunwoody</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Product3 Quantity</t>
+  </si>
+  <si>
+    <t>Product1 Quantity</t>
+  </si>
+  <si>
+    <t>Record Type of new record</t>
+  </si>
+  <si>
+    <t>Product1 Sales Price</t>
+  </si>
+  <si>
+    <t>Product2 Sales Price</t>
+  </si>
+  <si>
+    <t>Product3 Sales Price</t>
+  </si>
+  <si>
+    <t>Competitor Name</t>
+  </si>
+  <si>
+    <t>Competitor Strength</t>
+  </si>
+  <si>
+    <t>Competitor Weakness</t>
+  </si>
+  <si>
+    <t>Partner Name</t>
+  </si>
+  <si>
+    <t>Partner Role</t>
+  </si>
+  <si>
+    <t>Notes Title</t>
+  </si>
+  <si>
+    <t>Notes body</t>
+  </si>
+  <si>
+    <t>Test Notes Body</t>
+  </si>
+  <si>
+    <t>Test Automation Notes</t>
+  </si>
+  <si>
+    <t>Advertiser</t>
+  </si>
+  <si>
+    <t>Test Weakness</t>
+  </si>
+  <si>
+    <t>Test Strength</t>
+  </si>
+  <si>
+    <t>Test Competitor</t>
   </si>
 </sst>
 </file>
@@ -260,8 +398,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,7 +525,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -312,6 +538,50 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -324,6 +594,50 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -636,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -658,13 +972,13 @@
     <col min="13" max="13" width="9.83203125" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
     <col min="15" max="16" width="14.6640625" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" customWidth="1"/>
-    <col min="19" max="19" width="9.6640625" customWidth="1"/>
-    <col min="20" max="20" width="7.83203125" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" customWidth="1"/>
+    <col min="21" max="21" width="7.83203125" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="56">
+    <row r="1" spans="1:48" s="1" customFormat="1" ht="56">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +1016,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
@@ -717,69 +1031,105 @@
         <v>32</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="AG1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>59</v>
+      <c r="AK1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="1" customFormat="1" ht="42">
+    <row r="2" spans="1:48" s="1" customFormat="1" ht="42">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="1">
         <v>49898136</v>
@@ -809,7 +1159,7 @@
         <v>1000</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="1">
         <v>1</v>
@@ -824,64 +1174,100 @@
         <v>13</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="1">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="1">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="1">
+      <c r="V2" s="1">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1">
         <v>10</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="X2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="1">
-        <v>5</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>42818</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
         <v>10</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>42818</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>60</v>
+      <c r="AO2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -897,35 +1283,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:19" ht="56">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="28">
+    <row r="2" spans="1:19" ht="42">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="1">
+        <v>30090</v>
+      </c>
+      <c r="S2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added Test for role based login
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
+++ b/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Opportunity" sheetId="1" r:id="rId1"/>
-    <sheet name="Create New Dealer" sheetId="2" r:id="rId2"/>
+    <sheet name="Login Details" sheetId="4" r:id="rId1"/>
+    <sheet name="Create Opportunity" sheetId="1" r:id="rId2"/>
+    <sheet name="Create New Dealer" sheetId="2" r:id="rId3"/>
+    <sheet name="Login Roles" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="137">
   <si>
     <t>Username</t>
   </si>
@@ -350,6 +352,90 @@
   </si>
   <si>
     <t>Test Competitor</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Watkins, Zanea</t>
+  </si>
+  <si>
+    <t>Reed, Carolyn</t>
+  </si>
+  <si>
+    <t>Graham, Darby</t>
+  </si>
+  <si>
+    <t>Isom, Emilio</t>
+  </si>
+  <si>
+    <t>Levis, Ryan</t>
+  </si>
+  <si>
+    <t>Abulafi, Iyad</t>
+  </si>
+  <si>
+    <t>Jolitz, Maggie</t>
+  </si>
+  <si>
+    <t>Lichtenberger, Lydia</t>
+  </si>
+  <si>
+    <t>Assignee, Task</t>
+  </si>
+  <si>
+    <t>Augustaitis, George</t>
+  </si>
+  <si>
+    <t>Abrams, Randy</t>
+  </si>
+  <si>
+    <t>Brunson, Wendy</t>
+  </si>
+  <si>
+    <t>Augustine, Justin</t>
+  </si>
+  <si>
+    <t>Coordination Desk</t>
+  </si>
+  <si>
+    <t>Rewards Admin</t>
+  </si>
+  <si>
+    <t>All Sales, CAI Sales Ops</t>
+  </si>
+  <si>
+    <t>All Sales, CAI Sales</t>
+  </si>
+  <si>
+    <t>Reward Sales</t>
+  </si>
+  <si>
+    <t>Sales Engineer, CAI Sales</t>
+  </si>
+  <si>
+    <t>Business Admin:</t>
+  </si>
+  <si>
+    <t>CAI Admin</t>
+  </si>
+  <si>
+    <t>CAI Chatter Only</t>
+  </si>
+  <si>
+    <t>CAI Sales Ops Chatter</t>
+  </si>
+  <si>
+    <t>CAI Sales Chatter</t>
+  </si>
+  <si>
+    <t>CoE Viewer (Chatter Plus)</t>
+  </si>
+  <si>
+    <t>QA</t>
   </si>
 </sst>
 </file>
@@ -398,7 +484,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -511,6 +597,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
@@ -525,7 +620,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="122">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -582,6 +677,11 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -638,6 +738,10 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -950,10 +1054,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1281,12 +1421,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1424,4 +1564,141 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Tear Down method to capture exceptions
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
+++ b/src/test/resources/testdata/SalesforceUseCaseTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Login Details" sheetId="4" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>Account Name</t>
   </si>
   <si>
-    <t>TEST DEALER F</t>
-  </si>
-  <si>
     <t>Close Date</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>QA</t>
+  </si>
+  <si>
+    <t>SAM SWOPE BUICK GMC</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -605,6 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -620,7 +621,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -682,6 +683,7 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1046,7 +1048,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1072,10 +1074,10 @@
     </row>
     <row r="2" spans="1:2" ht="28">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1093,7 +1095,7 @@
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1156,7 +1158,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
@@ -1171,7 +1173,7 @@
         <v>32</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>33</v>
@@ -1186,7 +1188,7 @@
         <v>43</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>34</v>
@@ -1222,54 +1224,54 @@
         <v>51</v>
       </c>
       <c r="AI1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="AK1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" s="1" customFormat="1" ht="42">
+    </row>
+    <row r="2" spans="1:48" s="1" customFormat="1" ht="56">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>49898136</v>
@@ -1365,19 +1367,19 @@
         <v>48</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="AI2" s="3">
         <v>42818</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM2" s="1">
         <v>1</v>
@@ -1386,31 +1388,34 @@
         <v>10</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AH2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
@@ -1445,114 +1450,114 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="42">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="R2" s="1">
         <v>30090</v>
       </c>
       <c r="S2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1570,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1582,114 +1587,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
         <v>109</v>
-      </c>
-      <c r="B1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>